<commit_message>
Update to reproduction of Wang et al. (2024) results
Updated script to handle all columns read from the excel file.
</commit_message>
<xml_diff>
--- a/CaseStudy2_Wang2024/Outputs/Comparison_of_results.xlsx
+++ b/CaseStudy2_Wang2024/Outputs/Comparison_of_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://curtin-my.sharepoint.com/personal/283284g_curtin_edu_au/Documents/PycharmProjects/HierarchicalDataPaper/CaseStudy2_Wang2024/Outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="336" documentId="8_{B313DFBA-D778-4991-A51E-1A0F9AE2F1D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7588EFB-1342-4651-8C0D-ABE0FBA507A8}"/>
+  <xr:revisionPtr revIDLastSave="347" documentId="8_{B313DFBA-D778-4991-A51E-1A0F9AE2F1D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B8CAEF6-5AF4-4370-A7F6-1666E36DFC3C}"/>
   <bookViews>
-    <workbookView xWindow="32715" yWindow="435" windowWidth="21600" windowHeight="14865" xr2:uid="{04F0C4A7-3868-4D87-940A-6A2AA71C7693}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{04F0C4A7-3868-4D87-940A-6A2AA71C7693}"/>
   </bookViews>
   <sheets>
     <sheet name="Model metric comparison" sheetId="1" r:id="rId1"/>
@@ -326,51 +326,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -381,10 +370,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -401,6 +399,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -723,7 +725,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="A13" sqref="A13:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -740,41 +742,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="16"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -783,76 +785,76 @@
       <c r="C3" s="2">
         <v>0.94</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="23">
+        <v>0.94599999999999995</v>
+      </c>
       <c r="E3" s="3">
         <v>0.79600000000000004</v>
       </c>
       <c r="F3" s="3">
         <v>0.93799999999999994</v>
       </c>
-      <c r="G3" s="17"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
+      <c r="G3" s="10"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="22"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2">
         <v>0.91</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="23">
+        <v>0.90500000000000003</v>
+      </c>
       <c r="E4" s="3">
         <v>0.64100000000000001</v>
       </c>
       <c r="F4" s="3">
         <v>0.89200000000000002</v>
       </c>
-      <c r="G4" s="17"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
+      <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="22"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="2">
         <v>0.93</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="23">
+        <v>0.92500000000000004</v>
+      </c>
       <c r="E5" s="3">
         <v>0.71</v>
       </c>
       <c r="F5" s="3">
         <v>0.91500000000000004</v>
       </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
+      <c r="G5" s="10"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="23"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="2">
         <v>0.99</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="23">
+        <v>0.99199999999999999</v>
+      </c>
       <c r="E6" s="3">
         <v>0.90100000000000002</v>
       </c>
       <c r="F6" s="3">
         <v>0.99299999999999999</v>
       </c>
-      <c r="G6" s="17"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
+      <c r="G6" s="10"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -861,113 +863,113 @@
       <c r="C7" s="4">
         <v>0.94</v>
       </c>
-      <c r="D7" s="4"/>
+      <c r="D7" s="7">
+        <v>0.94299999999999995</v>
+      </c>
       <c r="E7" s="5">
         <v>0.78700000000000003</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="7">
         <v>0.94099999999999995</v>
       </c>
-      <c r="G7" s="17"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
+      <c r="G7" s="10"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="19"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="4">
         <v>0.91</v>
       </c>
-      <c r="D8" s="4"/>
+      <c r="D8" s="7">
+        <v>0.88600000000000001</v>
+      </c>
       <c r="E8" s="5">
         <v>0.622</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="7">
         <v>0.90900000000000003</v>
       </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
+      <c r="G8" s="10"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="19"/>
+      <c r="A9" s="20"/>
       <c r="B9" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="4">
         <v>0.93</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="7">
+        <v>0.91400000000000003</v>
+      </c>
       <c r="E9" s="5">
         <v>0.69499999999999995</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="7">
         <v>0.92500000000000004</v>
       </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
+      <c r="G9" s="10"/>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="20"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="4">
         <v>0.99</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="D10" s="7">
+        <v>0.99099999999999999</v>
+      </c>
       <c r="E10" s="5">
         <v>0.91900000000000004</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="7">
         <v>0.99399999999999999</v>
       </c>
-      <c r="G10" s="17"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-    </row>
-    <row r="11" spans="1:9" s="8" customFormat="1">
-      <c r="A11" s="24"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
+      <c r="G10" s="10"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
     </row>
     <row r="12" spans="1:9" ht="68.25" customHeight="1">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
     </row>
     <row r="13" spans="1:9" ht="83.25" customHeight="1">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
     </row>
     <row r="17" spans="3:3">
-      <c r="C17" s="13"/>
+      <c r="C17" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -1002,20 +1004,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="6"/>
+      <c r="D1" s="22"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
       <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
@@ -1030,10 +1032,10 @@
       <c r="B3" s="1">
         <v>0</v>
       </c>
-      <c r="C3" s="25">
-        <v>11705</v>
-      </c>
-      <c r="D3" s="25">
+      <c r="C3" s="1">
+        <v>11705</v>
+      </c>
+      <c r="D3" s="1">
         <v>11871</v>
       </c>
     </row>
@@ -1044,10 +1046,10 @@
       <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="C4" s="25">
-        <v>11705</v>
-      </c>
-      <c r="D4" s="25">
+      <c r="C4" s="1">
+        <v>11705</v>
+      </c>
+      <c r="D4" s="1">
         <v>11882</v>
       </c>
     </row>
@@ -1058,10 +1060,10 @@
       <c r="B5" s="1">
         <v>2</v>
       </c>
-      <c r="C5" s="25">
-        <v>11706</v>
-      </c>
-      <c r="D5" s="25">
+      <c r="C5" s="1">
+        <v>11706</v>
+      </c>
+      <c r="D5" s="1">
         <v>11332</v>
       </c>
     </row>
@@ -1072,10 +1074,10 @@
       <c r="B6" s="1">
         <v>3</v>
       </c>
-      <c r="C6" s="25">
-        <v>11706</v>
-      </c>
-      <c r="D6" s="25">
+      <c r="C6" s="1">
+        <v>11706</v>
+      </c>
+      <c r="D6" s="1">
         <v>11529</v>
       </c>
     </row>
@@ -1086,10 +1088,10 @@
       <c r="B7" s="1">
         <v>4</v>
       </c>
-      <c r="C7" s="25">
-        <v>11706</v>
-      </c>
-      <c r="D7" s="25">
+      <c r="C7" s="1">
+        <v>11706</v>
+      </c>
+      <c r="D7" s="1">
         <v>11742</v>
       </c>
     </row>
@@ -1101,10 +1103,10 @@
       <c r="B8" s="1">
         <v>0</v>
       </c>
-      <c r="C8" s="25">
-        <v>11705</v>
-      </c>
-      <c r="D8" s="25">
+      <c r="C8" s="1">
+        <v>11705</v>
+      </c>
+      <c r="D8" s="1">
         <v>11900</v>
       </c>
     </row>
@@ -1116,10 +1118,10 @@
       <c r="B9" s="1">
         <v>1</v>
       </c>
-      <c r="C9" s="25">
-        <v>11705</v>
-      </c>
-      <c r="D9" s="25">
+      <c r="C9" s="1">
+        <v>11705</v>
+      </c>
+      <c r="D9" s="1">
         <v>11368</v>
       </c>
     </row>
@@ -1131,10 +1133,10 @@
       <c r="B10" s="1">
         <v>2</v>
       </c>
-      <c r="C10" s="25">
-        <v>11706</v>
-      </c>
-      <c r="D10" s="25">
+      <c r="C10" s="1">
+        <v>11706</v>
+      </c>
+      <c r="D10" s="1">
         <v>11435</v>
       </c>
     </row>
@@ -1146,10 +1148,10 @@
       <c r="B11" s="1">
         <v>3</v>
       </c>
-      <c r="C11" s="25">
-        <v>11706</v>
-      </c>
-      <c r="D11" s="25">
+      <c r="C11" s="1">
+        <v>11706</v>
+      </c>
+      <c r="D11" s="1">
         <v>11914</v>
       </c>
     </row>
@@ -1161,10 +1163,10 @@
       <c r="B12" s="1">
         <v>4</v>
       </c>
-      <c r="C12" s="25">
-        <v>11706</v>
-      </c>
-      <c r="D12" s="25">
+      <c r="C12" s="1">
+        <v>11706</v>
+      </c>
+      <c r="D12" s="1">
         <v>11739</v>
       </c>
     </row>
@@ -1176,10 +1178,10 @@
       <c r="B13" s="1">
         <v>0</v>
       </c>
-      <c r="C13" s="25">
-        <v>11705</v>
-      </c>
-      <c r="D13" s="25">
+      <c r="C13" s="1">
+        <v>11705</v>
+      </c>
+      <c r="D13" s="1">
         <v>11483</v>
       </c>
     </row>
@@ -1191,10 +1193,10 @@
       <c r="B14" s="1">
         <v>1</v>
       </c>
-      <c r="C14" s="25">
-        <v>11705</v>
-      </c>
-      <c r="D14" s="25">
+      <c r="C14" s="1">
+        <v>11705</v>
+      </c>
+      <c r="D14" s="1">
         <v>11839</v>
       </c>
     </row>
@@ -1206,10 +1208,10 @@
       <c r="B15" s="1">
         <v>2</v>
       </c>
-      <c r="C15" s="25">
-        <v>11706</v>
-      </c>
-      <c r="D15" s="25">
+      <c r="C15" s="1">
+        <v>11706</v>
+      </c>
+      <c r="D15" s="1">
         <v>11609</v>
       </c>
     </row>
@@ -1221,10 +1223,10 @@
       <c r="B16" s="1">
         <v>3</v>
       </c>
-      <c r="C16" s="25">
-        <v>11706</v>
-      </c>
-      <c r="D16" s="25">
+      <c r="C16" s="1">
+        <v>11706</v>
+      </c>
+      <c r="D16" s="1">
         <v>11750</v>
       </c>
     </row>
@@ -1236,10 +1238,10 @@
       <c r="B17" s="1">
         <v>4</v>
       </c>
-      <c r="C17" s="25">
-        <v>11706</v>
-      </c>
-      <c r="D17" s="25">
+      <c r="C17" s="1">
+        <v>11706</v>
+      </c>
+      <c r="D17" s="1">
         <v>11675</v>
       </c>
     </row>
@@ -1251,10 +1253,10 @@
       <c r="B18" s="1">
         <v>0</v>
       </c>
-      <c r="C18" s="25">
-        <v>11705</v>
-      </c>
-      <c r="D18" s="25">
+      <c r="C18" s="1">
+        <v>11705</v>
+      </c>
+      <c r="D18" s="1">
         <v>11823</v>
       </c>
     </row>
@@ -1266,10 +1268,10 @@
       <c r="B19" s="1">
         <v>1</v>
       </c>
-      <c r="C19" s="25">
-        <v>11705</v>
-      </c>
-      <c r="D19" s="25">
+      <c r="C19" s="1">
+        <v>11705</v>
+      </c>
+      <c r="D19" s="1">
         <v>11578</v>
       </c>
     </row>
@@ -1281,10 +1283,10 @@
       <c r="B20" s="1">
         <v>2</v>
       </c>
-      <c r="C20" s="25">
-        <v>11706</v>
-      </c>
-      <c r="D20" s="25">
+      <c r="C20" s="1">
+        <v>11706</v>
+      </c>
+      <c r="D20" s="1">
         <v>11717</v>
       </c>
     </row>
@@ -1296,10 +1298,10 @@
       <c r="B21" s="1">
         <v>3</v>
       </c>
-      <c r="C21" s="25">
-        <v>11706</v>
-      </c>
-      <c r="D21" s="25">
+      <c r="C21" s="1">
+        <v>11706</v>
+      </c>
+      <c r="D21" s="1">
         <v>11577</v>
       </c>
     </row>
@@ -1311,10 +1313,10 @@
       <c r="B22" s="1">
         <v>4</v>
       </c>
-      <c r="C22" s="25">
-        <v>11706</v>
-      </c>
-      <c r="D22" s="25">
+      <c r="C22" s="1">
+        <v>11706</v>
+      </c>
+      <c r="D22" s="1">
         <v>11661</v>
       </c>
     </row>
@@ -1326,10 +1328,10 @@
       <c r="B23" s="1">
         <v>0</v>
       </c>
-      <c r="C23" s="25">
-        <v>11705</v>
-      </c>
-      <c r="D23" s="25">
+      <c r="C23" s="1">
+        <v>11705</v>
+      </c>
+      <c r="D23" s="1">
         <v>11734</v>
       </c>
     </row>
@@ -1341,10 +1343,10 @@
       <c r="B24" s="1">
         <v>1</v>
       </c>
-      <c r="C24" s="25">
-        <v>11705</v>
-      </c>
-      <c r="D24" s="25">
+      <c r="C24" s="1">
+        <v>11705</v>
+      </c>
+      <c r="D24" s="1">
         <v>11489</v>
       </c>
     </row>
@@ -1356,10 +1358,10 @@
       <c r="B25" s="1">
         <v>2</v>
       </c>
-      <c r="C25" s="25">
-        <v>11706</v>
-      </c>
-      <c r="D25" s="25">
+      <c r="C25" s="1">
+        <v>11706</v>
+      </c>
+      <c r="D25" s="1">
         <v>11661</v>
       </c>
     </row>
@@ -1371,10 +1373,10 @@
       <c r="B26" s="1">
         <v>3</v>
       </c>
-      <c r="C26" s="25">
-        <v>11706</v>
-      </c>
-      <c r="D26" s="25">
+      <c r="C26" s="1">
+        <v>11706</v>
+      </c>
+      <c r="D26" s="1">
         <v>11660</v>
       </c>
     </row>
@@ -1386,10 +1388,10 @@
       <c r="B27" s="1">
         <v>4</v>
       </c>
-      <c r="C27" s="25">
-        <v>11706</v>
-      </c>
-      <c r="D27" s="25">
+      <c r="C27" s="1">
+        <v>11706</v>
+      </c>
+      <c r="D27" s="1">
         <v>11812</v>
       </c>
     </row>
@@ -1401,10 +1403,10 @@
       <c r="B28" s="1">
         <v>0</v>
       </c>
-      <c r="C28" s="25">
-        <v>11705</v>
-      </c>
-      <c r="D28" s="25">
+      <c r="C28" s="1">
+        <v>11705</v>
+      </c>
+      <c r="D28" s="1">
         <v>11749</v>
       </c>
     </row>
@@ -1416,10 +1418,10 @@
       <c r="B29" s="1">
         <v>1</v>
       </c>
-      <c r="C29" s="25">
-        <v>11705</v>
-      </c>
-      <c r="D29" s="25">
+      <c r="C29" s="1">
+        <v>11705</v>
+      </c>
+      <c r="D29" s="1">
         <v>11559</v>
       </c>
     </row>
@@ -1431,10 +1433,10 @@
       <c r="B30" s="1">
         <v>2</v>
       </c>
-      <c r="C30" s="25">
-        <v>11706</v>
-      </c>
-      <c r="D30" s="25">
+      <c r="C30" s="1">
+        <v>11706</v>
+      </c>
+      <c r="D30" s="1">
         <v>11383</v>
       </c>
     </row>
@@ -1446,10 +1448,10 @@
       <c r="B31" s="1">
         <v>3</v>
       </c>
-      <c r="C31" s="25">
-        <v>11706</v>
-      </c>
-      <c r="D31" s="25">
+      <c r="C31" s="1">
+        <v>11706</v>
+      </c>
+      <c r="D31" s="1">
         <v>11751</v>
       </c>
     </row>
@@ -1461,10 +1463,10 @@
       <c r="B32" s="1">
         <v>4</v>
       </c>
-      <c r="C32" s="25">
-        <v>11706</v>
-      </c>
-      <c r="D32" s="25">
+      <c r="C32" s="1">
+        <v>11706</v>
+      </c>
+      <c r="D32" s="1">
         <v>11914</v>
       </c>
     </row>
@@ -1476,10 +1478,10 @@
       <c r="B33" s="1">
         <v>0</v>
       </c>
-      <c r="C33" s="25">
-        <v>11705</v>
-      </c>
-      <c r="D33" s="25">
+      <c r="C33" s="1">
+        <v>11705</v>
+      </c>
+      <c r="D33" s="1">
         <v>11970</v>
       </c>
     </row>
@@ -1491,10 +1493,10 @@
       <c r="B34" s="1">
         <v>1</v>
       </c>
-      <c r="C34" s="25">
-        <v>11705</v>
-      </c>
-      <c r="D34" s="25">
+      <c r="C34" s="1">
+        <v>11705</v>
+      </c>
+      <c r="D34" s="1">
         <v>11124</v>
       </c>
     </row>
@@ -1506,10 +1508,10 @@
       <c r="B35" s="1">
         <v>2</v>
       </c>
-      <c r="C35" s="25">
-        <v>11706</v>
-      </c>
-      <c r="D35" s="25">
+      <c r="C35" s="1">
+        <v>11706</v>
+      </c>
+      <c r="D35" s="1">
         <v>11577</v>
       </c>
     </row>
@@ -1521,10 +1523,10 @@
       <c r="B36" s="1">
         <v>3</v>
       </c>
-      <c r="C36" s="25">
-        <v>11706</v>
-      </c>
-      <c r="D36" s="25">
+      <c r="C36" s="1">
+        <v>11706</v>
+      </c>
+      <c r="D36" s="1">
         <v>11709</v>
       </c>
     </row>
@@ -1536,10 +1538,10 @@
       <c r="B37" s="1">
         <v>4</v>
       </c>
-      <c r="C37" s="25">
-        <v>11706</v>
-      </c>
-      <c r="D37" s="25">
+      <c r="C37" s="1">
+        <v>11706</v>
+      </c>
+      <c r="D37" s="1">
         <v>11976</v>
       </c>
     </row>
@@ -1551,10 +1553,10 @@
       <c r="B38" s="1">
         <v>0</v>
       </c>
-      <c r="C38" s="25">
-        <v>11705</v>
-      </c>
-      <c r="D38" s="25">
+      <c r="C38" s="1">
+        <v>11705</v>
+      </c>
+      <c r="D38" s="1">
         <v>11720</v>
       </c>
     </row>
@@ -1566,10 +1568,10 @@
       <c r="B39" s="1">
         <v>1</v>
       </c>
-      <c r="C39" s="25">
-        <v>11705</v>
-      </c>
-      <c r="D39" s="25">
+      <c r="C39" s="1">
+        <v>11705</v>
+      </c>
+      <c r="D39" s="1">
         <v>11405</v>
       </c>
     </row>
@@ -1581,10 +1583,10 @@
       <c r="B40" s="1">
         <v>2</v>
       </c>
-      <c r="C40" s="25">
-        <v>11706</v>
-      </c>
-      <c r="D40" s="25">
+      <c r="C40" s="1">
+        <v>11706</v>
+      </c>
+      <c r="D40" s="1">
         <v>11749</v>
       </c>
     </row>
@@ -1596,10 +1598,10 @@
       <c r="B41" s="1">
         <v>3</v>
       </c>
-      <c r="C41" s="25">
-        <v>11706</v>
-      </c>
-      <c r="D41" s="25">
+      <c r="C41" s="1">
+        <v>11706</v>
+      </c>
+      <c r="D41" s="1">
         <v>11803</v>
       </c>
     </row>
@@ -1611,10 +1613,10 @@
       <c r="B42" s="1">
         <v>4</v>
       </c>
-      <c r="C42" s="25">
-        <v>11706</v>
-      </c>
-      <c r="D42" s="25">
+      <c r="C42" s="1">
+        <v>11706</v>
+      </c>
+      <c r="D42" s="1">
         <v>11679</v>
       </c>
     </row>
@@ -1626,10 +1628,10 @@
       <c r="B43" s="1">
         <v>0</v>
       </c>
-      <c r="C43" s="25">
-        <v>11705</v>
-      </c>
-      <c r="D43" s="25">
+      <c r="C43" s="1">
+        <v>11705</v>
+      </c>
+      <c r="D43" s="1">
         <v>11462</v>
       </c>
     </row>
@@ -1641,10 +1643,10 @@
       <c r="B44" s="1">
         <v>1</v>
       </c>
-      <c r="C44" s="25">
-        <v>11705</v>
-      </c>
-      <c r="D44" s="25">
+      <c r="C44" s="1">
+        <v>11705</v>
+      </c>
+      <c r="D44" s="1">
         <v>11478</v>
       </c>
     </row>
@@ -1656,10 +1658,10 @@
       <c r="B45" s="1">
         <v>2</v>
       </c>
-      <c r="C45" s="25">
-        <v>11706</v>
-      </c>
-      <c r="D45" s="25">
+      <c r="C45" s="1">
+        <v>11706</v>
+      </c>
+      <c r="D45" s="1">
         <v>11819</v>
       </c>
     </row>
@@ -1671,10 +1673,10 @@
       <c r="B46" s="1">
         <v>3</v>
       </c>
-      <c r="C46" s="25">
-        <v>11706</v>
-      </c>
-      <c r="D46" s="25">
+      <c r="C46" s="1">
+        <v>11706</v>
+      </c>
+      <c r="D46" s="1">
         <v>11684</v>
       </c>
     </row>
@@ -1686,10 +1688,10 @@
       <c r="B47" s="1">
         <v>4</v>
       </c>
-      <c r="C47" s="25">
-        <v>11706</v>
-      </c>
-      <c r="D47" s="25">
+      <c r="C47" s="1">
+        <v>11706</v>
+      </c>
+      <c r="D47" s="1">
         <v>11913</v>
       </c>
     </row>
@@ -1701,10 +1703,10 @@
       <c r="B48" s="1">
         <v>0</v>
       </c>
-      <c r="C48" s="25">
-        <v>11705</v>
-      </c>
-      <c r="D48" s="25">
+      <c r="C48" s="1">
+        <v>11705</v>
+      </c>
+      <c r="D48" s="1">
         <v>12008</v>
       </c>
     </row>
@@ -1716,10 +1718,10 @@
       <c r="B49" s="1">
         <v>1</v>
       </c>
-      <c r="C49" s="25">
-        <v>11705</v>
-      </c>
-      <c r="D49" s="25">
+      <c r="C49" s="1">
+        <v>11705</v>
+      </c>
+      <c r="D49" s="1">
         <v>11554</v>
       </c>
     </row>
@@ -1731,10 +1733,10 @@
       <c r="B50" s="1">
         <v>2</v>
       </c>
-      <c r="C50" s="25">
-        <v>11706</v>
-      </c>
-      <c r="D50" s="25">
+      <c r="C50" s="1">
+        <v>11706</v>
+      </c>
+      <c r="D50" s="1">
         <v>11709</v>
       </c>
     </row>
@@ -1746,10 +1748,10 @@
       <c r="B51" s="1">
         <v>3</v>
       </c>
-      <c r="C51" s="25">
-        <v>11706</v>
-      </c>
-      <c r="D51" s="25">
+      <c r="C51" s="1">
+        <v>11706</v>
+      </c>
+      <c r="D51" s="1">
         <v>11684</v>
       </c>
     </row>
@@ -1761,10 +1763,10 @@
       <c r="B52" s="1">
         <v>4</v>
       </c>
-      <c r="C52" s="25">
-        <v>11706</v>
-      </c>
-      <c r="D52" s="25">
+      <c r="C52" s="1">
+        <v>11706</v>
+      </c>
+      <c r="D52" s="1">
         <v>11401</v>
       </c>
     </row>

</xml_diff>